<commit_message>
Add and fix skills
</commit_message>
<xml_diff>
--- a/skills/Redundant Skills.xlsx
+++ b/skills/Redundant Skills.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C7CA6-412D-0F49-83C3-EE42DA642799}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D23A50-991E-4E42-8D35-B8E7978AADE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12320" yWindow="460" windowWidth="16480" windowHeight="16180" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Skill</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>BASIC</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -173,8 +179,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A28" totalsRowShown="0">
-  <autoFilter ref="A1:A28" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A30" totalsRowShown="0">
+  <autoFilter ref="A1:A30" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
     <sortCondition ref="A1:A21"/>
   </sortState>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E914D5-27CD-7E41-A3B3-3B307D4A30A6}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,6 +639,16 @@
         <v>25</v>
       </c>
     </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Remove duplicate/spelling error skills
</commit_message>
<xml_diff>
--- a/skills/Redundant Skills.xlsx
+++ b/skills/Redundant Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D23A50-991E-4E42-8D35-B8E7978AADE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7209ED-9A6F-DB4B-87E1-A04970A7ECD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12320" yWindow="460" windowWidth="16480" windowHeight="16180" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
@@ -491,7 +491,7 @@
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>